<commit_message>
Allowed for multiple resources per room
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\r25excelgen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chase_000\Desktop\Git\r25excelgen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,7 +13,6 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$O$47</definedName>
@@ -2526,16 +2525,4 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added delivery and pickup times
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -945,23 +945,25 @@
   <dimension ref="A1:O76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="23.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9" style="3" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="3" customWidth="1"/>
-    <col min="10" max="11" width="18.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="3" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="14.5703125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="21.5703125" style="3" customWidth="1"/>
     <col min="15" max="15" width="16.42578125" style="3" customWidth="1"/>
     <col min="16" max="16384" width="12.85546875" style="1"/>
   </cols>

</xml_diff>